<commit_message>
/ ‘Iteration 2 comm/changes4polls.xlsx’
</commit_message>
<xml_diff>
--- a/Iteration 2 comm/changes4polls.xlsx
+++ b/Iteration 2 comm/changes4polls.xlsx
@@ -19,7 +19,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+  <si>
+    <t>poll_template_resultbody</t>
+  </si>
+  <si>
+    <t>&lt;li class="clearfix"&gt; &lt;span class="figures"&gt;%POLL_ANSWER_PERCENTAGE%%&lt;/span&gt; &lt;span class="info"&gt; &lt;div&gt;%POLL_ANSWER_TEXT%&lt;/div&gt; &lt;div class="bar" style="width:%POLL_ANSWER_PERCENTAGE%%;"&gt;&amp;nbsp;&lt;/div&gt; &lt;/span&gt; &lt;span class="figures"&gt;%POLL_ANSWER_VOTES%&lt;/span&gt; &lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>poll_template_resultbody2</t>
+  </si>
+  <si>
+    <t>poll_template_resultfooter</t>
+  </si>
   <si>
     <t>&lt;li class="clearfix"&gt; &lt;span class="figures"&gt;&amp;nbsp;&lt;/span&gt; &lt;span class="total"&gt;Total: %POLL_TOTALVOTERS% votes&lt;/span&gt; &lt;span class="figures"&gt;&amp;nbsp;&lt;/span&gt; &lt;/li&gt; &lt;/ul&gt; &lt;/section&gt;</t>
   </si>
@@ -63,9 +75,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;li class="clearfix"&gt; &lt;span class="figures"&gt;&amp;nbsp;&lt;/span&gt; &lt;span class="total"&gt;Total: %POLL_TOTALVOTERS% votes&lt;/span&gt; &lt;span class="figures"&gt;&amp;nbsp;&lt;/span&gt; &lt;/li&gt; &lt;/ul&gt; &lt;p style="text-align: center;"&gt;&lt;a href="#VotePoll" onclick="poll_booth(%POLL_ID%); return false;" title="Vote For This Poll"&gt;Vote&lt;/a&gt;&lt;/p&gt;&lt;/div&gt; &lt;/section&gt;</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -88,24 +97,18 @@
   </si>
   <si>
     <t>poll_template_resultheader</t>
-  </si>
-  <si>
-    <t>poll_template_resultbody</t>
-  </si>
-  <si>
-    <t>&lt;li class="clearfix"&gt; &lt;span class="figures"&gt;%POLL_ANSWER_PERCENTAGE%%&lt;/span&gt; &lt;span class="info"&gt; &lt;div&gt;%POLL_ANSWER_TEXT%&lt;/div&gt; &lt;div class="bar" style="width:%POLL_ANSWER_PERCENTAGE%%;"&gt;&amp;nbsp;&lt;/div&gt; &lt;/span&gt; &lt;span class="figures"&gt;%POLL_ANSWER_VOTES%&lt;/span&gt; &lt;/li&gt;</t>
-  </si>
-  <si>
-    <t>poll_template_resultbody2</t>
-  </si>
-  <si>
-    <t>poll_template_resultfooter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -481,7 +484,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -491,106 +494,107 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="52">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="65">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="39">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="52">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="65">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="65">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="78">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="78">
       <c r="A9" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>